<commit_message>
fixed first matchup issue
</commit_message>
<xml_diff>
--- a/proper.xlsx
+++ b/proper.xlsx
@@ -2137,11 +2137,11 @@
     <xf quotePrefix="1" borderId="23" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="13" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="22" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -13832,7 +13832,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13860,7 +13860,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13888,7 +13888,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13916,7 +13916,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -21390,7 +21390,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="39">
-        <f t="shared" ref="C4:C193" si="2">IFNA(INDEX(E:E, MATCH(B4, D:D, 0)), "")
+        <f t="shared" ref="C4:C46" si="2">IFNA(INDEX(E:E, MATCH(B4, D:D, 0)), "")
 </f>
         <v>29</v>
       </c>
@@ -22677,9 +22677,8 @@
       <c r="B47" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="39">
-        <f t="shared" si="2"/>
-        <v>1</v>
+      <c r="C47" s="53">
+        <v>2.0</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>155</v>
@@ -22703,7 +22702,8 @@
       <c r="A48" s="26"/>
       <c r="B48" s="48"/>
       <c r="C48" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C48:C193" si="3">IFNA(INDEX(E:E, MATCH(B48, D:D, 0)), "")
+</f>
         <v/>
       </c>
       <c r="D48" s="33" t="s">
@@ -22741,7 +22741,7 @@
         <v>261</v>
       </c>
       <c r="C49" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>218</v>
       </c>
       <c r="D49" s="50" t="s">
@@ -22768,7 +22768,7 @@
         <v>383</v>
       </c>
       <c r="C50" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="D50" s="45" t="s">
@@ -22793,7 +22793,7 @@
       <c r="A51" s="26"/>
       <c r="B51" s="48"/>
       <c r="C51" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D51" s="33" t="s">
@@ -22831,7 +22831,7 @@
         <v>349</v>
       </c>
       <c r="C52" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>171</v>
       </c>
       <c r="D52" s="50" t="s">
@@ -22858,7 +22858,7 @@
         <v>301</v>
       </c>
       <c r="C53" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>247</v>
       </c>
       <c r="D53" s="45" t="s">
@@ -22883,7 +22883,7 @@
       <c r="A54" s="26"/>
       <c r="B54" s="48"/>
       <c r="C54" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D54" s="33" t="s">
@@ -22921,7 +22921,7 @@
         <v>245</v>
       </c>
       <c r="C55" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199</v>
       </c>
       <c r="D55" s="50" t="s">
@@ -22948,7 +22948,7 @@
         <v>467</v>
       </c>
       <c r="C56" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>255</v>
       </c>
       <c r="D56" s="45" t="s">
@@ -22973,7 +22973,7 @@
       <c r="A57" s="26"/>
       <c r="B57" s="48"/>
       <c r="C57" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D57" s="33" t="s">
@@ -23011,7 +23011,7 @@
         <v>409</v>
       </c>
       <c r="C58" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>232</v>
       </c>
       <c r="D58" s="50" t="s">
@@ -23038,7 +23038,7 @@
         <v>389</v>
       </c>
       <c r="C59" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="D59" s="45" t="s">
@@ -23063,7 +23063,7 @@
       <c r="A60" s="26"/>
       <c r="B60" s="48"/>
       <c r="C60" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D60" s="33" t="s">
@@ -23101,7 +23101,7 @@
         <v>287</v>
       </c>
       <c r="C61" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>181</v>
       </c>
       <c r="D61" s="50" t="s">
@@ -23128,7 +23128,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>165</v>
       </c>
       <c r="D62" s="45" t="s">
@@ -23153,7 +23153,7 @@
       <c r="A63" s="26"/>
       <c r="B63" s="48"/>
       <c r="C63" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D63" s="33" t="s">
@@ -23191,7 +23191,7 @@
         <v>405</v>
       </c>
       <c r="C64" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="D64" s="50" t="s">
@@ -23218,7 +23218,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="D65" s="45" t="s">
@@ -23243,7 +23243,7 @@
       <c r="A66" s="26"/>
       <c r="B66" s="48"/>
       <c r="C66" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D66" s="33" t="s">
@@ -23281,7 +23281,7 @@
         <v>283</v>
       </c>
       <c r="C67" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="D67" s="50" t="s">
@@ -23308,7 +23308,7 @@
         <v>265</v>
       </c>
       <c r="C68" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="D68" s="45" t="s">
@@ -23333,7 +23333,7 @@
       <c r="A69" s="26"/>
       <c r="B69" s="48"/>
       <c r="C69" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D69" s="33" t="s">
@@ -23371,7 +23371,7 @@
         <v>431</v>
       </c>
       <c r="C70" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
       <c r="D70" s="50" t="s">
@@ -23398,7 +23398,7 @@
         <v>85</v>
       </c>
       <c r="C71" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="D71" s="45" t="s">
@@ -23423,7 +23423,7 @@
       <c r="A72" s="26"/>
       <c r="B72" s="48"/>
       <c r="C72" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D72" s="33" t="s">
@@ -23461,7 +23461,7 @@
         <v>99</v>
       </c>
       <c r="C73" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>158</v>
       </c>
       <c r="D73" s="50" t="s">
@@ -23488,7 +23488,7 @@
         <v>381</v>
       </c>
       <c r="C74" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="D74" s="45" t="s">
@@ -23513,7 +23513,7 @@
       <c r="A75" s="26"/>
       <c r="B75" s="48"/>
       <c r="C75" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D75" s="33" t="s">
@@ -23551,7 +23551,7 @@
         <v>47</v>
       </c>
       <c r="C76" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
       <c r="D76" s="50" t="s">
@@ -23578,7 +23578,7 @@
         <v>157</v>
       </c>
       <c r="C77" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="D77" s="45" t="s">
@@ -23603,7 +23603,7 @@
       <c r="A78" s="26"/>
       <c r="B78" s="48"/>
       <c r="C78" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D78" s="33" t="s">
@@ -23641,7 +23641,7 @@
         <v>469</v>
       </c>
       <c r="C79" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>164</v>
       </c>
       <c r="D79" s="50" t="s">
@@ -23668,7 +23668,7 @@
         <v>407</v>
       </c>
       <c r="C80" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="D80" s="45" t="s">
@@ -23693,7 +23693,7 @@
       <c r="A81" s="26"/>
       <c r="B81" s="48"/>
       <c r="C81" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D81" s="33" t="s">
@@ -23731,7 +23731,7 @@
         <v>461</v>
       </c>
       <c r="C82" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="D82" s="50" t="s">
@@ -23758,7 +23758,7 @@
         <v>327</v>
       </c>
       <c r="C83" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="D83" s="45" t="s">
@@ -23783,7 +23783,7 @@
       <c r="A84" s="26"/>
       <c r="B84" s="48"/>
       <c r="C84" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D84" s="33" t="s">
@@ -23821,7 +23821,7 @@
         <v>59</v>
       </c>
       <c r="C85" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>223</v>
       </c>
       <c r="D85" s="50" t="s">
@@ -23848,7 +23848,7 @@
         <v>97</v>
       </c>
       <c r="C86" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>213</v>
       </c>
       <c r="D86" s="45" t="s">
@@ -23873,7 +23873,7 @@
       <c r="A87" s="26"/>
       <c r="B87" s="48"/>
       <c r="C87" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D87" s="33" t="s">
@@ -23911,7 +23911,7 @@
         <v>504</v>
       </c>
       <c r="C88" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="D88" s="50" t="s">
@@ -23938,7 +23938,7 @@
         <v>181</v>
       </c>
       <c r="C89" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="D89" s="45" t="s">
@@ -23963,7 +23963,7 @@
       <c r="A90" s="26"/>
       <c r="B90" s="48"/>
       <c r="C90" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D90" s="33" t="s">
@@ -24001,7 +24001,7 @@
         <v>121</v>
       </c>
       <c r="C91" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>249</v>
       </c>
       <c r="D91" s="50" t="s">
@@ -24028,7 +24028,7 @@
         <v>335</v>
       </c>
       <c r="C92" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="D92" s="45" t="s">
@@ -24053,7 +24053,7 @@
       <c r="A93" s="26"/>
       <c r="B93" s="48"/>
       <c r="C93" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D93" s="33" t="s">
@@ -24091,7 +24091,7 @@
         <v>525</v>
       </c>
       <c r="C94" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="D94" s="50" t="s">
@@ -24118,7 +24118,7 @@
         <v>91</v>
       </c>
       <c r="C95" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="D95" s="45" t="s">
@@ -24143,7 +24143,7 @@
       <c r="A96" s="26"/>
       <c r="B96" s="48"/>
       <c r="C96" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D96" s="33" t="s">
@@ -24181,7 +24181,7 @@
         <v>131</v>
       </c>
       <c r="C97" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="D97" s="50" t="s">
@@ -24208,7 +24208,7 @@
         <v>255</v>
       </c>
       <c r="C98" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>257</v>
       </c>
       <c r="D98" s="45" t="s">
@@ -24233,7 +24233,7 @@
       <c r="A99" s="26"/>
       <c r="B99" s="48"/>
       <c r="C99" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D99" s="33" t="s">
@@ -24271,7 +24271,7 @@
         <v>421</v>
       </c>
       <c r="C100" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="D100" s="50" t="s">
@@ -24298,7 +24298,7 @@
         <v>393</v>
       </c>
       <c r="C101" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>173</v>
       </c>
       <c r="D101" s="45" t="s">
@@ -24323,7 +24323,7 @@
       <c r="A102" s="26"/>
       <c r="B102" s="48"/>
       <c r="C102" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D102" s="33" t="s">
@@ -24361,7 +24361,7 @@
         <v>17</v>
       </c>
       <c r="C103" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="D103" s="50" t="s">
@@ -24388,7 +24388,7 @@
         <v>247</v>
       </c>
       <c r="C104" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="D104" s="45" t="s">
@@ -24413,7 +24413,7 @@
       <c r="A105" s="26"/>
       <c r="B105" s="48"/>
       <c r="C105" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D105" s="33" t="s">
@@ -24451,7 +24451,7 @@
         <v>125</v>
       </c>
       <c r="C106" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>251</v>
       </c>
       <c r="D106" s="50" t="s">
@@ -24478,7 +24478,7 @@
         <v>473</v>
       </c>
       <c r="C107" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="D107" s="45" t="s">
@@ -24503,7 +24503,7 @@
       <c r="A108" s="26"/>
       <c r="B108" s="48"/>
       <c r="C108" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D108" s="33" t="s">
@@ -24541,7 +24541,7 @@
         <v>213</v>
       </c>
       <c r="C109" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="D109" s="50" t="s">
@@ -24568,7 +24568,7 @@
         <v>175</v>
       </c>
       <c r="C110" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="D110" s="45" t="s">
@@ -24593,7 +24593,7 @@
       <c r="A111" s="26"/>
       <c r="B111" s="48"/>
       <c r="C111" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D111" s="33" t="s">
@@ -24631,7 +24631,7 @@
         <v>15</v>
       </c>
       <c r="C112" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>147</v>
       </c>
       <c r="D112" s="50" t="s">
@@ -24658,7 +24658,7 @@
         <v>31</v>
       </c>
       <c r="C113" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="D113" s="45" t="s">
@@ -24683,7 +24683,7 @@
       <c r="A114" s="26"/>
       <c r="B114" s="48"/>
       <c r="C114" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D114" s="33" t="s">
@@ -24721,7 +24721,7 @@
         <v>496</v>
       </c>
       <c r="C115" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="D115" s="50" t="s">
@@ -24748,7 +24748,7 @@
         <v>161</v>
       </c>
       <c r="C116" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D116" s="45" t="s">
@@ -24773,7 +24773,7 @@
       <c r="A117" s="26"/>
       <c r="B117" s="48"/>
       <c r="C117" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D117" s="33" t="s">
@@ -24811,7 +24811,7 @@
         <v>55</v>
       </c>
       <c r="C118" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159</v>
       </c>
       <c r="D118" s="50" t="s">
@@ -24838,7 +24838,7 @@
         <v>357</v>
       </c>
       <c r="C119" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="D119" s="45" t="s">
@@ -24863,7 +24863,7 @@
       <c r="A120" s="26"/>
       <c r="B120" s="48"/>
       <c r="C120" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D120" s="33" t="s">
@@ -24901,7 +24901,7 @@
         <v>429</v>
       </c>
       <c r="C121" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D121" s="50" t="s">
@@ -24928,7 +24928,7 @@
         <v>141</v>
       </c>
       <c r="C122" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="D122" s="45" t="s">
@@ -24953,7 +24953,7 @@
       <c r="A123" s="26"/>
       <c r="B123" s="48"/>
       <c r="C123" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D123" s="33" t="s">
@@ -24991,7 +24991,7 @@
         <v>518</v>
       </c>
       <c r="C124" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="D124" s="50" t="s">
@@ -25018,7 +25018,7 @@
         <v>435</v>
       </c>
       <c r="C125" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>155</v>
       </c>
       <c r="D125" s="45" t="s">
@@ -25043,7 +25043,7 @@
       <c r="A126" s="26"/>
       <c r="B126" s="48"/>
       <c r="C126" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D126" s="33" t="s">
@@ -25081,7 +25081,7 @@
         <v>103</v>
       </c>
       <c r="C127" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="D127" s="50" t="s">
@@ -25108,7 +25108,7 @@
         <v>514</v>
       </c>
       <c r="C128" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>231</v>
       </c>
       <c r="D128" s="45" t="s">
@@ -25133,7 +25133,7 @@
       <c r="A129" s="26"/>
       <c r="B129" s="48"/>
       <c r="C129" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D129" s="33" t="s">
@@ -25171,7 +25171,7 @@
         <v>269</v>
       </c>
       <c r="C130" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="D130" s="50" t="s">
@@ -25198,7 +25198,7 @@
         <v>169</v>
       </c>
       <c r="C131" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
       <c r="D131" s="45" t="s">
@@ -25223,7 +25223,7 @@
       <c r="A132" s="26"/>
       <c r="B132" s="48"/>
       <c r="C132" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D132" s="33" t="s">
@@ -25261,7 +25261,7 @@
         <v>305</v>
       </c>
       <c r="C133" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="D133" s="50" t="s">
@@ -25288,7 +25288,7 @@
         <v>73</v>
       </c>
       <c r="C134" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="D134" s="45" t="s">
@@ -25313,7 +25313,7 @@
       <c r="A135" s="26"/>
       <c r="B135" s="48"/>
       <c r="C135" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D135" s="33" t="s">
@@ -25351,7 +25351,7 @@
         <v>325</v>
       </c>
       <c r="C136" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="D136" s="50" t="s">
@@ -25378,7 +25378,7 @@
         <v>187</v>
       </c>
       <c r="C137" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>214</v>
       </c>
       <c r="D137" s="45" t="s">
@@ -25403,7 +25403,7 @@
       <c r="A138" s="26"/>
       <c r="B138" s="48"/>
       <c r="C138" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D138" s="33" t="s">
@@ -25441,7 +25441,7 @@
         <v>487</v>
       </c>
       <c r="C139" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="D139" s="50" t="s">
@@ -25468,7 +25468,7 @@
         <v>463</v>
       </c>
       <c r="C140" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="D140" s="45" t="s">
@@ -25493,7 +25493,7 @@
       <c r="A141" s="26"/>
       <c r="B141" s="48"/>
       <c r="C141" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D141" s="33" t="s">
@@ -25531,7 +25531,7 @@
         <v>207</v>
       </c>
       <c r="C142" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>188</v>
       </c>
       <c r="D142" s="50" t="s">
@@ -25558,7 +25558,7 @@
         <v>75</v>
       </c>
       <c r="C143" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="D143" s="45" t="s">
@@ -25583,7 +25583,7 @@
       <c r="A144" s="26"/>
       <c r="B144" s="48"/>
       <c r="C144" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D144" s="33" t="s">
@@ -25621,7 +25621,7 @@
         <v>149</v>
       </c>
       <c r="C145" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>162</v>
       </c>
       <c r="D145" s="50" t="s">
@@ -25648,7 +25648,7 @@
         <v>483</v>
       </c>
       <c r="C146" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="D146" s="45" t="s">
@@ -25673,7 +25673,7 @@
       <c r="A147" s="26"/>
       <c r="B147" s="48"/>
       <c r="C147" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D147" s="33" t="s">
@@ -25711,7 +25711,7 @@
         <v>127</v>
       </c>
       <c r="C148" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
       <c r="D148" s="50" t="s">
@@ -25738,7 +25738,7 @@
         <v>63</v>
       </c>
       <c r="C149" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="D149" s="45" t="s">
@@ -25763,7 +25763,7 @@
       <c r="A150" s="26"/>
       <c r="B150" s="48"/>
       <c r="C150" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D150" s="33" t="s">
@@ -25801,7 +25801,7 @@
         <v>203</v>
       </c>
       <c r="C151" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="D151" s="50" t="s">
@@ -25828,7 +25828,7 @@
         <v>395</v>
       </c>
       <c r="C152" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="D152" s="45" t="s">
@@ -25853,7 +25853,7 @@
       <c r="A153" s="26"/>
       <c r="B153" s="48"/>
       <c r="C153" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D153" s="33" t="s">
@@ -25891,7 +25891,7 @@
         <v>385</v>
       </c>
       <c r="C154" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="D154" s="50" t="s">
@@ -25918,7 +25918,7 @@
         <v>451</v>
       </c>
       <c r="C155" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>221</v>
       </c>
       <c r="D155" s="45" t="s">
@@ -25943,7 +25943,7 @@
       <c r="A156" s="26"/>
       <c r="B156" s="48"/>
       <c r="C156" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D156" s="33" t="s">
@@ -25981,10 +25981,10 @@
         <v>163</v>
       </c>
       <c r="C157" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
-      <c r="D157" s="53" t="s">
+      <c r="D157" s="54" t="s">
         <v>528</v>
       </c>
       <c r="E157" s="41">
@@ -26008,7 +26008,7 @@
         <v>363</v>
       </c>
       <c r="C158" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="D158" s="45" t="s">
@@ -26033,7 +26033,7 @@
       <c r="A159" s="26"/>
       <c r="B159" s="48"/>
       <c r="C159" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D159" s="33" t="s">
@@ -26071,7 +26071,7 @@
         <v>165</v>
       </c>
       <c r="C160" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="D160" s="50" t="s">
@@ -26098,7 +26098,7 @@
         <v>129</v>
       </c>
       <c r="C161" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="D161" s="45" t="s">
@@ -26123,7 +26123,7 @@
       <c r="A162" s="26"/>
       <c r="B162" s="48"/>
       <c r="C162" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D162" s="33" t="s">
@@ -26161,7 +26161,7 @@
         <v>87</v>
       </c>
       <c r="C163" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="D163" s="50" t="s">
@@ -26188,7 +26188,7 @@
         <v>411</v>
       </c>
       <c r="C164" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="D164" s="45" t="s">
@@ -26213,7 +26213,7 @@
       <c r="A165" s="26"/>
       <c r="B165" s="48"/>
       <c r="C165" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D165" s="33" t="s">
@@ -26251,7 +26251,7 @@
         <v>527</v>
       </c>
       <c r="C166" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="D166" s="50" t="s">
@@ -26278,7 +26278,7 @@
         <v>492</v>
       </c>
       <c r="C167" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="D167" s="45" t="s">
@@ -26303,7 +26303,7 @@
       <c r="A168" s="26"/>
       <c r="B168" s="48"/>
       <c r="C168" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D168" s="33" t="s">
@@ -26341,7 +26341,7 @@
         <v>19</v>
       </c>
       <c r="C169" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="D169" s="50" t="s">
@@ -26368,7 +26368,7 @@
         <v>29</v>
       </c>
       <c r="C170" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="D170" s="45" t="s">
@@ -26393,7 +26393,7 @@
       <c r="A171" s="26"/>
       <c r="B171" s="48"/>
       <c r="C171" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D171" s="33" t="s">
@@ -26431,7 +26431,7 @@
         <v>520</v>
       </c>
       <c r="C172" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D172" s="50" t="s">
@@ -26458,7 +26458,7 @@
         <v>433</v>
       </c>
       <c r="C173" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>183</v>
       </c>
       <c r="D173" s="45" t="s">
@@ -26483,7 +26483,7 @@
       <c r="A174" s="26"/>
       <c r="B174" s="48"/>
       <c r="C174" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D174" s="33" t="s">
@@ -26521,7 +26521,7 @@
         <v>415</v>
       </c>
       <c r="C175" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>168</v>
       </c>
       <c r="D175" s="50" t="s">
@@ -26548,7 +26548,7 @@
         <v>397</v>
       </c>
       <c r="C176" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="D176" s="45" t="s">
@@ -26573,7 +26573,7 @@
       <c r="A177" s="26"/>
       <c r="B177" s="48"/>
       <c r="C177" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D177" s="33" t="s">
@@ -26611,7 +26611,7 @@
         <v>291</v>
       </c>
       <c r="C178" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="D178" s="50" t="s">
@@ -26638,7 +26638,7 @@
         <v>35</v>
       </c>
       <c r="C179" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="D179" s="45" t="s">
@@ -26663,7 +26663,7 @@
       <c r="A180" s="26"/>
       <c r="B180" s="48"/>
       <c r="C180" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D180" s="33" t="s">
@@ -26701,7 +26701,7 @@
         <v>3</v>
       </c>
       <c r="C181" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>202</v>
       </c>
       <c r="D181" s="50" t="s">
@@ -26728,7 +26728,7 @@
         <v>39</v>
       </c>
       <c r="C182" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="D182" s="45" t="s">
@@ -26753,7 +26753,7 @@
       <c r="A183" s="26"/>
       <c r="B183" s="48"/>
       <c r="C183" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D183" s="33" t="s">
@@ -26791,7 +26791,7 @@
         <v>371</v>
       </c>
       <c r="C184" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="D184" s="50" t="s">
@@ -26818,7 +26818,7 @@
         <v>359</v>
       </c>
       <c r="C185" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="D185" s="45" t="s">
@@ -26843,7 +26843,7 @@
       <c r="A186" s="26"/>
       <c r="B186" s="48"/>
       <c r="C186" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D186" s="33" t="s">
@@ -26881,7 +26881,7 @@
         <v>191</v>
       </c>
       <c r="C187" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="D187" s="50" t="s">
@@ -26908,7 +26908,7 @@
         <v>263</v>
       </c>
       <c r="C188" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D188" s="45" t="s">
@@ -26933,7 +26933,7 @@
       <c r="A189" s="26"/>
       <c r="B189" s="48"/>
       <c r="C189" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D189" s="33" t="s">
@@ -26971,7 +26971,7 @@
         <v>37</v>
       </c>
       <c r="C190" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="D190" s="50" t="s">
@@ -26998,7 +26998,7 @@
         <v>437</v>
       </c>
       <c r="C191" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="D191" s="45" t="s">
@@ -27023,7 +27023,7 @@
       <c r="A192" s="26"/>
       <c r="B192" s="48"/>
       <c r="C192" s="39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D192" s="33" t="s">
@@ -27061,7 +27061,7 @@
         <v>13</v>
       </c>
       <c r="C193" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="D193" s="50" t="s">
@@ -27087,7 +27087,7 @@
       <c r="B194" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="C194" s="54">
+      <c r="C194" s="53">
         <v>190.0</v>
       </c>
       <c r="D194" s="45" t="s">
@@ -27112,7 +27112,7 @@
       <c r="A195" s="26"/>
       <c r="B195" s="48"/>
       <c r="C195" s="39" t="str">
-        <f t="shared" ref="C195:C295" si="3">IFNA(INDEX(E:E, MATCH(B195, D:D, 0)), "")
+        <f t="shared" ref="C195:C211" si="4">IFNA(INDEX(E:E, MATCH(B195, D:D, 0)), "")
 </f>
         <v/>
       </c>
@@ -27151,7 +27151,7 @@
         <v>189</v>
       </c>
       <c r="C196" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131</v>
       </c>
       <c r="D196" s="50" t="s">
@@ -27178,7 +27178,7 @@
         <v>439</v>
       </c>
       <c r="C197" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
       <c r="D197" s="45" t="s">
@@ -27203,7 +27203,7 @@
       <c r="A198" s="26"/>
       <c r="B198" s="48"/>
       <c r="C198" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D198" s="33" t="s">
@@ -27241,7 +27241,7 @@
         <v>377</v>
       </c>
       <c r="C199" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="D199" s="50" t="s">
@@ -27268,7 +27268,7 @@
         <v>485</v>
       </c>
       <c r="C200" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
       <c r="D200" s="45" t="s">
@@ -27293,7 +27293,7 @@
       <c r="A201" s="26"/>
       <c r="B201" s="48"/>
       <c r="C201" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D201" s="33" t="s">
@@ -27331,7 +27331,7 @@
         <v>117</v>
       </c>
       <c r="C202" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="D202" s="50" t="s">
@@ -27358,7 +27358,7 @@
         <v>481</v>
       </c>
       <c r="C203" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>216</v>
       </c>
       <c r="D203" s="45" t="s">
@@ -27383,7 +27383,7 @@
       <c r="A204" s="26"/>
       <c r="B204" s="48"/>
       <c r="C204" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D204" s="33" t="s">
@@ -27421,7 +27421,7 @@
         <v>259</v>
       </c>
       <c r="C205" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>177</v>
       </c>
       <c r="D205" s="50" t="s">
@@ -27448,7 +27448,7 @@
         <v>183</v>
       </c>
       <c r="C206" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="D206" s="45" t="s">
@@ -27473,7 +27473,7 @@
       <c r="A207" s="26"/>
       <c r="B207" s="48"/>
       <c r="C207" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D207" s="33" t="s">
@@ -27511,7 +27511,7 @@
         <v>417</v>
       </c>
       <c r="C208" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="D208" s="50" t="s">
@@ -27538,7 +27538,7 @@
         <v>205</v>
       </c>
       <c r="C209" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="D209" s="45" t="s">
@@ -27563,7 +27563,7 @@
       <c r="A210" s="26"/>
       <c r="B210" s="48"/>
       <c r="C210" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="D210" s="33" t="s">
@@ -27601,7 +27601,7 @@
         <v>193</v>
       </c>
       <c r="C211" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="D211" s="50" t="s">
@@ -27627,9 +27627,8 @@
       <c r="B212" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="C212" s="39">
-        <f t="shared" si="3"/>
-        <v>2</v>
+      <c r="C212" s="53">
+        <v>1.0</v>
       </c>
       <c r="D212" s="45" t="s">
         <v>494</v>
@@ -27653,7 +27652,8 @@
       <c r="A213" s="26"/>
       <c r="B213" s="48"/>
       <c r="C213" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C213:C295" si="5">IFNA(INDEX(E:E, MATCH(B213, D:D, 0)), "")
+</f>
         <v/>
       </c>
       <c r="D213" s="33" t="s">
@@ -27691,7 +27691,7 @@
         <v>445</v>
       </c>
       <c r="C214" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="D214" s="50" t="s">
@@ -27718,7 +27718,7 @@
         <v>199</v>
       </c>
       <c r="C215" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="D215" s="45" t="s">
@@ -27743,7 +27743,7 @@
       <c r="A216" s="26"/>
       <c r="B216" s="48"/>
       <c r="C216" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D216" s="33" t="s">
@@ -27781,7 +27781,7 @@
         <v>179</v>
       </c>
       <c r="C217" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="D217" s="50" t="s">
@@ -27808,7 +27808,7 @@
         <v>173</v>
       </c>
       <c r="C218" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="D218" s="45" t="s">
@@ -27833,7 +27833,7 @@
       <c r="A219" s="26"/>
       <c r="B219" s="48"/>
       <c r="C219" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D219" s="33" t="s">
@@ -27871,7 +27871,7 @@
         <v>494</v>
       </c>
       <c r="C220" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>212</v>
       </c>
       <c r="D220" s="50" t="s">
@@ -27898,7 +27898,7 @@
         <v>93</v>
       </c>
       <c r="C221" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="D221" s="45" t="s">
@@ -27923,7 +27923,7 @@
       <c r="A222" s="26"/>
       <c r="B222" s="48"/>
       <c r="C222" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D222" s="33" t="s">
@@ -27961,7 +27961,7 @@
         <v>273</v>
       </c>
       <c r="C223" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="D223" s="50" t="s">
@@ -27988,7 +27988,7 @@
         <v>369</v>
       </c>
       <c r="C224" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
       <c r="D224" s="45" t="s">
@@ -28013,7 +28013,7 @@
       <c r="A225" s="26"/>
       <c r="B225" s="48"/>
       <c r="C225" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D225" s="33" t="s">
@@ -28051,7 +28051,7 @@
         <v>143</v>
       </c>
       <c r="C226" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D226" s="50" t="s">
@@ -28078,7 +28078,7 @@
         <v>453</v>
       </c>
       <c r="C227" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="D227" s="45" t="s">
@@ -28103,7 +28103,7 @@
       <c r="A228" s="26"/>
       <c r="B228" s="48"/>
       <c r="C228" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D228" s="33" t="s">
@@ -28141,7 +28141,7 @@
         <v>171</v>
       </c>
       <c r="C229" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>62</v>
       </c>
       <c r="D229" s="50" t="s">
@@ -28168,7 +28168,7 @@
         <v>477</v>
       </c>
       <c r="C230" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>245</v>
       </c>
       <c r="D230" s="45" t="s">
@@ -28193,7 +28193,7 @@
       <c r="A231" s="26"/>
       <c r="B231" s="48"/>
       <c r="C231" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D231" s="33" t="s">
@@ -28231,7 +28231,7 @@
         <v>11</v>
       </c>
       <c r="C232" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="D232" s="50" t="s">
@@ -28258,7 +28258,7 @@
         <v>113</v>
       </c>
       <c r="C233" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>228</v>
       </c>
       <c r="D233" s="45" t="s">
@@ -28283,7 +28283,7 @@
       <c r="A234" s="26"/>
       <c r="B234" s="48"/>
       <c r="C234" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D234" s="33" t="s">
@@ -28321,7 +28321,7 @@
         <v>449</v>
       </c>
       <c r="C235" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>205</v>
       </c>
       <c r="D235" s="50" t="s">
@@ -28348,7 +28348,7 @@
         <v>457</v>
       </c>
       <c r="C236" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153</v>
       </c>
       <c r="D236" s="45" t="s">
@@ -28373,7 +28373,7 @@
       <c r="A237" s="26"/>
       <c r="B237" s="48"/>
       <c r="C237" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D237" s="33" t="s">
@@ -28411,7 +28411,7 @@
         <v>45</v>
       </c>
       <c r="C238" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>260</v>
       </c>
       <c r="D238" s="50" t="s">
@@ -28438,7 +28438,7 @@
         <v>508</v>
       </c>
       <c r="C239" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="D239" s="45" t="s">
@@ -28463,7 +28463,7 @@
       <c r="A240" s="26"/>
       <c r="B240" s="48"/>
       <c r="C240" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D240" s="33" t="s">
@@ -28501,7 +28501,7 @@
         <v>81</v>
       </c>
       <c r="C241" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="D241" s="50" t="s">
@@ -28528,7 +28528,7 @@
         <v>139</v>
       </c>
       <c r="C242" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="D242" s="45" t="s">
@@ -28553,7 +28553,7 @@
       <c r="A243" s="26"/>
       <c r="B243" s="48"/>
       <c r="C243" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D243" s="33" t="s">
@@ -28591,7 +28591,7 @@
         <v>281</v>
       </c>
       <c r="C244" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>101</v>
       </c>
       <c r="D244" s="50" t="s">
@@ -28618,7 +28618,7 @@
         <v>43</v>
       </c>
       <c r="C245" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>125</v>
       </c>
       <c r="D245" s="45" t="s">
@@ -28643,7 +28643,7 @@
       <c r="A246" s="26"/>
       <c r="B246" s="48"/>
       <c r="C246" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D246" s="33" t="s">
@@ -28681,7 +28681,7 @@
         <v>53</v>
       </c>
       <c r="C247" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="D247" s="50" t="s">
@@ -28708,7 +28708,7 @@
         <v>317</v>
       </c>
       <c r="C248" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>236</v>
       </c>
       <c r="D248" s="45" t="s">
@@ -28733,7 +28733,7 @@
       <c r="A249" s="26"/>
       <c r="B249" s="48"/>
       <c r="C249" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D249" s="33" t="s">
@@ -28771,7 +28771,7 @@
         <v>79</v>
       </c>
       <c r="C250" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>248</v>
       </c>
       <c r="D250" s="50" t="s">
@@ -28798,7 +28798,7 @@
         <v>516</v>
       </c>
       <c r="C251" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D251" s="45" t="s">
@@ -28823,7 +28823,7 @@
       <c r="A252" s="26"/>
       <c r="B252" s="48"/>
       <c r="C252" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D252" s="33" t="s">
@@ -28861,7 +28861,7 @@
         <v>219</v>
       </c>
       <c r="C253" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>241</v>
       </c>
       <c r="D253" s="50" t="s">
@@ -28888,7 +28888,7 @@
         <v>315</v>
       </c>
       <c r="C254" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="D254" s="45" t="s">
@@ -28913,7 +28913,7 @@
       <c r="A255" s="26"/>
       <c r="B255" s="48"/>
       <c r="C255" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D255" s="33" t="s">
@@ -28951,7 +28951,7 @@
         <v>167</v>
       </c>
       <c r="C256" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="D256" s="50" t="s">
@@ -28978,7 +28978,7 @@
         <v>379</v>
       </c>
       <c r="C257" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="D257" s="45" t="s">
@@ -29003,7 +29003,7 @@
       <c r="A258" s="26"/>
       <c r="B258" s="48"/>
       <c r="C258" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D258" s="33" t="s">
@@ -29041,7 +29041,7 @@
         <v>311</v>
       </c>
       <c r="C259" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="D259" s="50" t="s">
@@ -29068,7 +29068,7 @@
         <v>341</v>
       </c>
       <c r="C260" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="D260" s="45" t="s">
@@ -29093,7 +29093,7 @@
       <c r="A261" s="26"/>
       <c r="B261" s="48"/>
       <c r="C261" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D261" s="55"/>
@@ -29126,7 +29126,7 @@
         <v>147</v>
       </c>
       <c r="C262" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>239</v>
       </c>
       <c r="D262" s="57"/>
@@ -29148,7 +29148,7 @@
         <v>297</v>
       </c>
       <c r="C263" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>211</v>
       </c>
       <c r="D263" s="59"/>
@@ -29168,7 +29168,7 @@
       <c r="A264" s="26"/>
       <c r="B264" s="48"/>
       <c r="C264" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D264" s="55"/>
@@ -29201,7 +29201,7 @@
         <v>177</v>
       </c>
       <c r="C265" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>133</v>
       </c>
       <c r="D265" s="57"/>
@@ -29223,7 +29223,7 @@
         <v>498</v>
       </c>
       <c r="C266" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="D266" s="59"/>
@@ -29243,7 +29243,7 @@
       <c r="A267" s="26"/>
       <c r="B267" s="48"/>
       <c r="C267" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D267" s="55"/>
@@ -29276,7 +29276,7 @@
         <v>123</v>
       </c>
       <c r="C268" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>256</v>
       </c>
       <c r="D268" s="57"/>
@@ -29298,7 +29298,7 @@
         <v>49</v>
       </c>
       <c r="C269" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D269" s="59"/>
@@ -29318,7 +29318,7 @@
       <c r="A270" s="26"/>
       <c r="B270" s="48"/>
       <c r="C270" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D270" s="55"/>
@@ -29351,7 +29351,7 @@
         <v>355</v>
       </c>
       <c r="C271" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>243</v>
       </c>
       <c r="D271" s="57"/>
@@ -29373,7 +29373,7 @@
         <v>529</v>
       </c>
       <c r="C272" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>259</v>
       </c>
       <c r="D272" s="59"/>
@@ -29393,7 +29393,7 @@
       <c r="A273" s="26"/>
       <c r="B273" s="48"/>
       <c r="C273" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D273" s="55"/>
@@ -29426,7 +29426,7 @@
         <v>506</v>
       </c>
       <c r="C274" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>201</v>
       </c>
       <c r="D274" s="57"/>
@@ -29448,7 +29448,7 @@
         <v>271</v>
       </c>
       <c r="C275" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>246</v>
       </c>
       <c r="D275" s="59"/>
@@ -29468,7 +29468,7 @@
       <c r="A276" s="26"/>
       <c r="B276" s="48"/>
       <c r="C276" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D276" s="55"/>
@@ -29501,7 +29501,7 @@
         <v>293</v>
       </c>
       <c r="C277" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>237</v>
       </c>
       <c r="D277" s="57"/>
@@ -29523,7 +29523,7 @@
         <v>423</v>
       </c>
       <c r="C278" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="D278" s="59"/>
@@ -29543,7 +29543,7 @@
       <c r="A279" s="26"/>
       <c r="B279" s="48"/>
       <c r="C279" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D279" s="55"/>
@@ -29576,7 +29576,7 @@
         <v>9</v>
       </c>
       <c r="C280" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="D280" s="57"/>
@@ -29598,7 +29598,7 @@
         <v>231</v>
       </c>
       <c r="C281" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="D281" s="59"/>
@@ -29618,7 +29618,7 @@
       <c r="A282" s="26"/>
       <c r="B282" s="48"/>
       <c r="C282" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D282" s="55"/>
@@ -29651,7 +29651,7 @@
         <v>217</v>
       </c>
       <c r="C283" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>242</v>
       </c>
       <c r="D283" s="57"/>
@@ -29673,7 +29673,7 @@
         <v>151</v>
       </c>
       <c r="C284" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="D284" s="59"/>
@@ -29693,7 +29693,7 @@
       <c r="A285" s="26"/>
       <c r="B285" s="48"/>
       <c r="C285" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D285" s="55"/>
@@ -29726,7 +29726,7 @@
         <v>277</v>
       </c>
       <c r="C286" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>230</v>
       </c>
       <c r="D286" s="57"/>
@@ -29748,7 +29748,7 @@
         <v>95</v>
       </c>
       <c r="C287" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>252</v>
       </c>
       <c r="D287" s="59"/>
@@ -29768,7 +29768,7 @@
       <c r="A288" s="26"/>
       <c r="B288" s="48"/>
       <c r="C288" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D288" s="55"/>
@@ -29801,7 +29801,7 @@
         <v>307</v>
       </c>
       <c r="C289" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="D289" s="57"/>
@@ -29823,7 +29823,7 @@
         <v>329</v>
       </c>
       <c r="C290" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>229</v>
       </c>
       <c r="D290" s="59"/>
@@ -29843,7 +29843,7 @@
       <c r="A291" s="26"/>
       <c r="B291" s="48"/>
       <c r="C291" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D291" s="55"/>
@@ -29876,7 +29876,7 @@
         <v>251</v>
       </c>
       <c r="C292" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="D292" s="57"/>
@@ -29898,7 +29898,7 @@
         <v>89</v>
       </c>
       <c r="C293" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="D293" s="59"/>
@@ -29918,7 +29918,7 @@
       <c r="A294" s="26"/>
       <c r="B294" s="48"/>
       <c r="C294" s="39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D294" s="55"/>
@@ -29951,7 +29951,7 @@
         <v>221</v>
       </c>
       <c r="C295" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>220</v>
       </c>
       <c r="D295" s="57"/>
@@ -29972,7 +29972,7 @@
       <c r="B296" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="C296" s="54">
+      <c r="C296" s="53">
         <v>189.0</v>
       </c>
       <c r="D296" s="59"/>
@@ -29992,7 +29992,7 @@
       <c r="A297" s="26"/>
       <c r="B297" s="48"/>
       <c r="C297" s="39" t="str">
-        <f t="shared" ref="C297:C379" si="4">IFNA(INDEX(E:E, MATCH(B297, D:D, 0)), "")
+        <f t="shared" ref="C297:C379" si="6">IFNA(INDEX(E:E, MATCH(B297, D:D, 0)), "")
 </f>
         <v/>
       </c>
@@ -30026,7 +30026,7 @@
         <v>241</v>
       </c>
       <c r="C298" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="D298" s="57"/>
@@ -30048,7 +30048,7 @@
         <v>65</v>
       </c>
       <c r="C299" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="D299" s="59"/>
@@ -30068,7 +30068,7 @@
       <c r="A300" s="26"/>
       <c r="B300" s="48"/>
       <c r="C300" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D300" s="55"/>
@@ -30101,7 +30101,7 @@
         <v>528</v>
       </c>
       <c r="C301" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>157</v>
       </c>
       <c r="D301" s="57"/>
@@ -30123,7 +30123,7 @@
         <v>135</v>
       </c>
       <c r="C302" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>169</v>
       </c>
       <c r="D302" s="59"/>
@@ -30143,7 +30143,7 @@
       <c r="A303" s="26"/>
       <c r="B303" s="48"/>
       <c r="C303" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D303" s="55"/>
@@ -30176,7 +30176,7 @@
         <v>343</v>
       </c>
       <c r="C304" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>235</v>
       </c>
       <c r="D304" s="57"/>
@@ -30198,7 +30198,7 @@
         <v>109</v>
       </c>
       <c r="C305" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="D305" s="59"/>
@@ -30218,7 +30218,7 @@
       <c r="A306" s="26"/>
       <c r="B306" s="48"/>
       <c r="C306" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D306" s="55"/>
@@ -30251,7 +30251,7 @@
         <v>133</v>
       </c>
       <c r="C307" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>215</v>
       </c>
       <c r="D307" s="57"/>
@@ -30273,7 +30273,7 @@
         <v>155</v>
       </c>
       <c r="C308" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="D308" s="59"/>
@@ -30293,7 +30293,7 @@
       <c r="A309" s="26"/>
       <c r="B309" s="48"/>
       <c r="C309" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D309" s="55"/>
@@ -30326,7 +30326,7 @@
         <v>321</v>
       </c>
       <c r="C310" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="D310" s="57"/>
@@ -30348,7 +30348,7 @@
         <v>351</v>
       </c>
       <c r="C311" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="D311" s="59"/>
@@ -30368,7 +30368,7 @@
       <c r="A312" s="26"/>
       <c r="B312" s="48"/>
       <c r="C312" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D312" s="55"/>
@@ -30401,7 +30401,7 @@
         <v>71</v>
       </c>
       <c r="C313" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="D313" s="57"/>
@@ -30423,7 +30423,7 @@
         <v>289</v>
       </c>
       <c r="C314" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>156</v>
       </c>
       <c r="D314" s="59"/>
@@ -30443,7 +30443,7 @@
       <c r="A315" s="26"/>
       <c r="B315" s="48"/>
       <c r="C315" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D315" s="55"/>
@@ -30476,7 +30476,7 @@
         <v>526</v>
       </c>
       <c r="C316" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="D316" s="57"/>
@@ -30498,7 +30498,7 @@
         <v>237</v>
       </c>
       <c r="C317" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>244</v>
       </c>
       <c r="D317" s="59"/>
@@ -30518,7 +30518,7 @@
       <c r="A318" s="26"/>
       <c r="B318" s="48"/>
       <c r="C318" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D318" s="55"/>
@@ -30551,7 +30551,7 @@
         <v>500</v>
       </c>
       <c r="C319" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="D319" s="57"/>
@@ -30573,7 +30573,7 @@
         <v>309</v>
       </c>
       <c r="C320" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>152</v>
       </c>
       <c r="D320" s="59"/>
@@ -30593,7 +30593,7 @@
       <c r="A321" s="26"/>
       <c r="B321" s="48"/>
       <c r="C321" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D321" s="55"/>
@@ -30626,7 +30626,7 @@
         <v>159</v>
       </c>
       <c r="C322" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>129</v>
       </c>
       <c r="D322" s="57"/>
@@ -30648,7 +30648,7 @@
         <v>23</v>
       </c>
       <c r="C323" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>97</v>
       </c>
       <c r="D323" s="59"/>
@@ -30668,7 +30668,7 @@
       <c r="A324" s="26"/>
       <c r="B324" s="48"/>
       <c r="C324" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D324" s="55"/>
@@ -30701,7 +30701,7 @@
         <v>339</v>
       </c>
       <c r="C325" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>108</v>
       </c>
       <c r="D325" s="57"/>
@@ -30723,7 +30723,7 @@
         <v>243</v>
       </c>
       <c r="C326" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D326" s="59"/>
@@ -30743,7 +30743,7 @@
       <c r="A327" s="26"/>
       <c r="B327" s="48"/>
       <c r="C327" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D327" s="55"/>
@@ -30776,7 +30776,7 @@
         <v>83</v>
       </c>
       <c r="C328" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>121</v>
       </c>
       <c r="D328" s="57"/>
@@ -30798,7 +30798,7 @@
         <v>249</v>
       </c>
       <c r="C329" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="D329" s="59"/>
@@ -30818,7 +30818,7 @@
       <c r="A330" s="26"/>
       <c r="B330" s="48"/>
       <c r="C330" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D330" s="55"/>
@@ -30851,7 +30851,7 @@
         <v>267</v>
       </c>
       <c r="C331" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="D331" s="57"/>
@@ -30873,7 +30873,7 @@
         <v>225</v>
       </c>
       <c r="C332" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>114</v>
       </c>
       <c r="D332" s="59"/>
@@ -30893,7 +30893,7 @@
       <c r="A333" s="26"/>
       <c r="B333" s="48"/>
       <c r="C333" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D333" s="55"/>
@@ -30926,7 +30926,7 @@
         <v>475</v>
       </c>
       <c r="C334" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>119</v>
       </c>
       <c r="D334" s="57"/>
@@ -30948,7 +30948,7 @@
         <v>229</v>
       </c>
       <c r="C335" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>175</v>
       </c>
       <c r="D335" s="59"/>
@@ -30968,7 +30968,7 @@
       <c r="A336" s="26"/>
       <c r="B336" s="48"/>
       <c r="C336" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D336" s="55"/>
@@ -31001,7 +31001,7 @@
         <v>227</v>
       </c>
       <c r="C337" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="D337" s="57"/>
@@ -31023,7 +31023,7 @@
         <v>375</v>
       </c>
       <c r="C338" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="D338" s="59"/>
@@ -31043,7 +31043,7 @@
       <c r="A339" s="26"/>
       <c r="B339" s="48"/>
       <c r="C339" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D339" s="55"/>
@@ -31076,7 +31076,7 @@
         <v>223</v>
       </c>
       <c r="C340" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>219</v>
       </c>
       <c r="D340" s="57"/>
@@ -31098,7 +31098,7 @@
         <v>185</v>
       </c>
       <c r="C341" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>139</v>
       </c>
       <c r="D341" s="59"/>
@@ -31118,7 +31118,7 @@
       <c r="A342" s="26"/>
       <c r="B342" s="48"/>
       <c r="C342" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D342" s="55"/>
@@ -31151,7 +31151,7 @@
         <v>447</v>
       </c>
       <c r="C343" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>225</v>
       </c>
       <c r="D343" s="57"/>
@@ -31173,7 +31173,7 @@
         <v>333</v>
       </c>
       <c r="C344" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="D344" s="59"/>
@@ -31193,7 +31193,7 @@
       <c r="A345" s="26"/>
       <c r="B345" s="48"/>
       <c r="C345" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D345" s="55"/>
@@ -31226,7 +31226,7 @@
         <v>490</v>
       </c>
       <c r="C346" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>103</v>
       </c>
       <c r="D346" s="57"/>
@@ -31248,7 +31248,7 @@
         <v>471</v>
       </c>
       <c r="C347" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>193</v>
       </c>
       <c r="D347" s="59"/>
@@ -31268,7 +31268,7 @@
       <c r="A348" s="26"/>
       <c r="B348" s="48"/>
       <c r="C348" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D348" s="55"/>
@@ -31301,7 +31301,7 @@
         <v>413</v>
       </c>
       <c r="C349" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>112</v>
       </c>
       <c r="D349" s="57"/>
@@ -31323,7 +31323,7 @@
         <v>387</v>
       </c>
       <c r="C350" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="D350" s="59"/>
@@ -31343,7 +31343,7 @@
       <c r="A351" s="26"/>
       <c r="B351" s="48"/>
       <c r="C351" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D351" s="55"/>
@@ -31376,7 +31376,7 @@
         <v>367</v>
       </c>
       <c r="C352" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>122</v>
       </c>
       <c r="D352" s="57"/>
@@ -31398,7 +31398,7 @@
         <v>441</v>
       </c>
       <c r="C353" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="D353" s="59"/>
@@ -31418,7 +31418,7 @@
       <c r="A354" s="26"/>
       <c r="B354" s="48"/>
       <c r="C354" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D354" s="55"/>
@@ -31451,7 +31451,7 @@
         <v>69</v>
       </c>
       <c r="C355" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>227</v>
       </c>
       <c r="D355" s="57"/>
@@ -31473,7 +31473,7 @@
         <v>111</v>
       </c>
       <c r="C356" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>233</v>
       </c>
       <c r="D356" s="59"/>
@@ -31493,7 +31493,7 @@
       <c r="A357" s="26"/>
       <c r="B357" s="48"/>
       <c r="C357" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D357" s="55"/>
@@ -31526,7 +31526,7 @@
         <v>119</v>
       </c>
       <c r="C358" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="D358" s="57"/>
@@ -31548,7 +31548,7 @@
         <v>479</v>
       </c>
       <c r="C359" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>178</v>
       </c>
       <c r="D359" s="59"/>
@@ -31568,7 +31568,7 @@
       <c r="A360" s="26"/>
       <c r="B360" s="48"/>
       <c r="C360" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D360" s="55"/>
@@ -31601,7 +31601,7 @@
         <v>391</v>
       </c>
       <c r="C361" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>185</v>
       </c>
       <c r="D361" s="57"/>
@@ -31623,7 +31623,7 @@
         <v>465</v>
       </c>
       <c r="C362" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="D362" s="59"/>
@@ -31643,7 +31643,7 @@
       <c r="A363" s="26"/>
       <c r="B363" s="48"/>
       <c r="C363" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D363" s="55"/>
@@ -31676,7 +31676,7 @@
         <v>51</v>
       </c>
       <c r="C364" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="D364" s="57"/>
@@ -31698,7 +31698,7 @@
         <v>361</v>
       </c>
       <c r="C365" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>124</v>
       </c>
       <c r="D365" s="59"/>
@@ -31718,7 +31718,7 @@
       <c r="A366" s="26"/>
       <c r="B366" s="48"/>
       <c r="C366" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D366" s="55"/>
@@ -31751,7 +31751,7 @@
         <v>512</v>
       </c>
       <c r="C367" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>148</v>
       </c>
       <c r="D367" s="57"/>
@@ -31773,7 +31773,7 @@
         <v>459</v>
       </c>
       <c r="C368" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>206</v>
       </c>
       <c r="D368" s="59"/>
@@ -31793,7 +31793,7 @@
       <c r="A369" s="26"/>
       <c r="B369" s="48"/>
       <c r="C369" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D369" s="55"/>
@@ -31826,7 +31826,7 @@
         <v>115</v>
       </c>
       <c r="C370" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="D370" s="57"/>
@@ -31848,7 +31848,7 @@
         <v>347</v>
       </c>
       <c r="C371" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>179</v>
       </c>
       <c r="D371" s="59"/>
@@ -31868,7 +31868,7 @@
       <c r="A372" s="26"/>
       <c r="B372" s="48"/>
       <c r="C372" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D372" s="55"/>
@@ -31901,7 +31901,7 @@
         <v>303</v>
       </c>
       <c r="C373" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="D373" s="57"/>
@@ -31923,7 +31923,7 @@
         <v>353</v>
       </c>
       <c r="C374" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="D374" s="59"/>
@@ -31943,7 +31943,7 @@
       <c r="A375" s="26"/>
       <c r="B375" s="48"/>
       <c r="C375" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D375" s="55"/>
@@ -31976,7 +31976,7 @@
         <v>401</v>
       </c>
       <c r="C376" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="D376" s="57"/>
@@ -31998,7 +31998,7 @@
         <v>319</v>
       </c>
       <c r="C377" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
       <c r="D377" s="59"/>
@@ -32018,7 +32018,7 @@
       <c r="A378" s="26"/>
       <c r="B378" s="48"/>
       <c r="C378" s="39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D378" s="55"/>
@@ -32051,7 +32051,7 @@
         <v>365</v>
       </c>
       <c r="C379" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>253</v>
       </c>
       <c r="D379" s="57"/>
@@ -32072,7 +32072,7 @@
       <c r="B380" s="51" t="s">
         <v>319</v>
       </c>
-      <c r="C380" s="54">
+      <c r="C380" s="53">
         <v>192.0</v>
       </c>
       <c r="D380" s="59"/>
@@ -32092,7 +32092,7 @@
       <c r="A381" s="26"/>
       <c r="B381" s="48"/>
       <c r="C381" s="39" t="str">
-        <f t="shared" ref="C381:C392" si="5">IFNA(INDEX(E:E, MATCH(B381, D:D, 0)), "")
+        <f t="shared" ref="C381:C392" si="7">IFNA(INDEX(E:E, MATCH(B381, D:D, 0)), "")
 </f>
         <v/>
       </c>
@@ -32126,7 +32126,7 @@
         <v>67</v>
       </c>
       <c r="C382" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="D382" s="57"/>
@@ -32148,7 +32148,7 @@
         <v>295</v>
       </c>
       <c r="C383" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>86</v>
       </c>
       <c r="D383" s="59"/>
@@ -32168,7 +32168,7 @@
       <c r="A384" s="26"/>
       <c r="B384" s="48"/>
       <c r="C384" s="39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D384" s="55"/>
@@ -32201,7 +32201,7 @@
         <v>275</v>
       </c>
       <c r="C385" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="D385" s="57"/>
@@ -32223,7 +32223,7 @@
         <v>57</v>
       </c>
       <c r="C386" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>209</v>
       </c>
       <c r="D386" s="59"/>
@@ -32243,7 +32243,7 @@
       <c r="A387" s="26"/>
       <c r="B387" s="48"/>
       <c r="C387" s="39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D387" s="55"/>
@@ -32276,7 +32276,7 @@
         <v>285</v>
       </c>
       <c r="C388" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>105</v>
       </c>
       <c r="D388" s="57"/>
@@ -32298,7 +32298,7 @@
         <v>101</v>
       </c>
       <c r="C389" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="D389" s="59"/>
@@ -32318,7 +32318,7 @@
       <c r="A390" s="26"/>
       <c r="B390" s="48"/>
       <c r="C390" s="39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="D390" s="55"/>
@@ -32351,7 +32351,7 @@
         <v>77</v>
       </c>
       <c r="C391" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>174</v>
       </c>
       <c r="D391" s="57"/>
@@ -32373,7 +32373,7 @@
         <v>373</v>
       </c>
       <c r="C392" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>170</v>
       </c>
       <c r="D392" s="59"/>

</xml_diff>

<commit_message>
Updated schedule for Round 2 Knockout
</commit_message>
<xml_diff>
--- a/proper.xlsx
+++ b/proper.xlsx
@@ -13832,7 +13832,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image3.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13860,7 +13860,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13888,7 +13888,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -13916,7 +13916,7 @@
     <xdr:ext cx="885825" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>